<commit_message>
Fix WHEN scoring to properly flag vague timing as missing
</commit_message>
<xml_diff>
--- a/Control_Test_Data2.xlsx
+++ b/Control_Test_Data2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee8d3d5c28cf10e6/Desktop/Python/Scripts/Attempt3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee8d3d5c28cf10e6/Desktop/final_consolidated_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_EAC61CD997D9AECF8A160B43F39EDB81722244FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9869F47-95C7-4D43-B4E2-AB4A27D88D5C}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_EAC61CD997D9AECF8A160B43F39EDB81722244FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E8AE1FC-7027-42A0-81E6-BFE66560A245}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38490" yWindow="1980" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Control_ID</t>
   </si>
@@ -67,9 +67,6 @@
     <t>CTRL-010</t>
   </si>
   <si>
-    <t>The IAM system automatically disables user accounts after 90 consecutive days of inactivity. A scheduled job runs daily to assess login activity.</t>
-  </si>
-  <si>
     <t>Each day, the system generates a report of inactive accounts. The IT Security Administrator reviews it and disables them if needed.</t>
   </si>
   <si>
@@ -140,6 +137,15 @@
   </si>
   <si>
     <t>Tariq Lee</t>
+  </si>
+  <si>
+    <t>The Accounting Manager reviews monthly bank reconciliations prepared by the Senior Accountant to ensure completeness and accuracy. Reconciliations are completed by the 5th business day. Unresolved items over $1,000 are escalated to the Controller.</t>
+  </si>
+  <si>
+    <t>CTRL-011</t>
+  </si>
+  <si>
+    <t>On a monthly basis, the Finance Accounts Receivable Manager reviews delinquent balances over 120 days old to verify compliance with the Company's write-off policy and regulatory requirements. The manager validates that all qualifying accounts have been properly identified for write-off by comparing the aged receivables report against established thresholds. Any accounts incorrectly processed are documented, and discrepancies exceeding $10,000 are escalated to the Finance Accounts Receivable Director for resolution.</t>
   </si>
 </sst>
 </file>
@@ -218,6 +224,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,16 +554,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -561,16 +571,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -578,16 +588,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -595,16 +605,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,16 +622,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -629,16 +639,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -646,16 +656,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -663,16 +673,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,16 +690,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -697,16 +707,33 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>37</v>
+      <c r="E12" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>